<commit_message>
Added test data sheets for Fireclass Belgium market
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_PanelNode_Repeaters_P_Panels.xlsx
+++ b/Test Data/Gallery_PanelNode_Repeaters_P_Panels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEA4A6A-1B3E-455D-8D82-4401223EFA25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D4FD19-8F37-4ED5-B1C3-B566DD57BD9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Swiss" sheetId="14" r:id="rId4"/>
     <sheet name="Portugal" sheetId="15" r:id="rId5"/>
     <sheet name="Slovakia" sheetId="16" r:id="rId6"/>
-    <sheet name="Itlay" sheetId="17" r:id="rId7"/>
+    <sheet name="Italy" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1487,7 +1487,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>